<commit_message>
Carico Modello Fisico + alcune modifice dd
</commit_message>
<xml_diff>
--- a/Registro/Data_Dictionary/tbl_Registro_individuale_v1.xlsx
+++ b/Registro/Data_Dictionary/tbl_Registro_individuale_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Desktop\ITS Tech Talent Factory\Materiale del corso\Basi di Dati\DATABASE-FSD1\Registro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Desktop\ITS Tech Talent Factory\Materiale del corso\Basi di Dati\DATABASE-FSD1\Registro\Data_Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9530ED94-488C-47F1-926D-75217A9C373C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF29D38-74C9-4BF4-ABC9-8B1B627C803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A13CAFEC-9B05-48C3-A700-6122505BF81D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A13CAFEC-9B05-48C3-A700-6122505BF81D}"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>VARCHAR(16)</t>
   </si>
   <si>
-    <t>VARCHAR(10)</t>
-  </si>
-  <si>
     <t>TIME</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>SMALLINT(5)</t>
+  </si>
+  <si>
+    <t>CHAR(10)</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B3C40F-E4BE-4F03-A053-01B1B734AC68}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="152" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +623,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="9" t="s">
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8"/>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -824,7 +824,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,12 +853,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -881,7 +881,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -890,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -898,14 +898,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -913,14 +913,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -935,7 +935,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -983,16 +983,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -1087,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4C928B-048C-4EF6-AF7D-12893DE3E5DC}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1214,7 +1214,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -1246,7 +1246,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Aggiungo orario_inizio/termine lezione + mf index
</commit_message>
<xml_diff>
--- a/Registro/Data_Dictionary/tbl_Registro_individuale_v1.xlsx
+++ b/Registro/Data_Dictionary/tbl_Registro_individuale_v1.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Desktop\ITS Tech Talent Factory\Materiale del corso\Basi di Dati\DATABASE-FSD1\Registro\Data_Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF29D38-74C9-4BF4-ABC9-8B1B627C803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C97886-1773-4864-B04D-BC62C4CAA3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A13CAFEC-9B05-48C3-A700-6122505BF81D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{A13CAFEC-9B05-48C3-A700-6122505BF81D}"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO" sheetId="1" r:id="rId1"/>
     <sheet name="PRESENZA" sheetId="3" r:id="rId2"/>
     <sheet name="FIRMA" sheetId="6" r:id="rId3"/>
     <sheet name="STUDENTE" sheetId="4" r:id="rId4"/>
-    <sheet name="DOCENTE" sheetId="5" r:id="rId5"/>
-    <sheet name="LEZIONE" sheetId="7" r:id="rId6"/>
+    <sheet name="LEZIONE" sheetId="7" r:id="rId5"/>
+    <sheet name="DOCENTE" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="43">
   <si>
     <t>Campo</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Argomento</t>
   </si>
   <si>
-    <t>Orario</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>CHAR(10)</t>
+  </si>
+  <si>
+    <t>Orario_termine</t>
+  </si>
+  <si>
+    <t>Orario_inizio</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -623,7 +626,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -638,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -651,32 +654,32 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="8"/>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="8"/>
     </row>
@@ -689,46 +692,46 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="8"/>
     </row>
@@ -789,7 +792,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -797,14 +800,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -853,12 +856,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -873,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -881,7 +884,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -890,7 +893,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -898,14 +901,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -913,14 +916,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -928,14 +931,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -983,16 +986,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1007,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1020,20 +1023,20 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -1043,6 +1046,160 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4C928B-048C-4EF6-AF7D-12893DE3E5DC}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCBC4A6-84DC-4697-A438-6282ACE23149}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1078,7 +1235,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1087,7 +1244,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -1102,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1115,148 +1272,24 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4C928B-048C-4EF6-AF7D-12893DE3E5DC}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>